<commit_message>
Creacion de areas comunales, falta eliminar y detalles
</commit_message>
<xml_diff>
--- a/Prueba Datos Sistema.xlsx
+++ b/Prueba Datos Sistema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VisualStudio\Personal\Roberto-Conjuntos\ProyectoConjuntos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual\Proyecto_Roberto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90190648-6A3C-4497-BE0F-ECCF3EDDA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C6A16F-C5EC-4C7E-B1B0-46E2EE33CABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -54,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{B60A89FA-E3C6-4F29-8E9D-03DB2895267F}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{B60A89FA-E3C6-4F29-8E9D-03DB2895267F}">
       <text>
         <r>
           <rPr>
@@ -83,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Ingreso</t>
   </si>
@@ -127,9 +138,6 @@
     <t># Comprobante</t>
   </si>
   <si>
-    <t>Mes</t>
-  </si>
-  <si>
     <t>Concepto</t>
   </si>
   <si>
@@ -151,9 +159,6 @@
     <t>Adeudos Por cobrar</t>
   </si>
   <si>
-    <t>Propietarios/Arendatarios</t>
-  </si>
-  <si>
     <t>PEDRO SANDOVAL</t>
   </si>
   <si>
@@ -197,6 +202,51 @@
   </si>
   <si>
     <t>Pago de Pedro Sandoval</t>
+  </si>
+  <si>
+    <t>Mes+secuencial</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Bancos</t>
+  </si>
+  <si>
+    <t># 1</t>
+  </si>
+  <si>
+    <t># 2</t>
+  </si>
+  <si>
+    <t># 3</t>
+  </si>
+  <si>
+    <t># 4</t>
+  </si>
+  <si>
+    <t>CAJA</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Deposito</t>
+  </si>
+  <si>
+    <t>Efectivo de Pedro Sandoval</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>Alicuotas</t>
+  </si>
+  <si>
+    <t>11020101</t>
+  </si>
+  <si>
+    <t>Ctas.por Cobrar Clientes</t>
   </si>
 </sst>
 </file>
@@ -241,10 +291,39 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -253,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +356,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,34 +692,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A3F21E-1B0E-4FCA-92AD-C360CB3777B3}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:G32"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="8"/>
       <c r="F1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -626,13 +727,26 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="12" t="str">
+        <f>G7</f>
+        <v>Alicuotas</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="12"/>
+      <c r="O2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="12"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -643,50 +757,120 @@
         <v>111</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="14">
+        <f>F24</f>
+        <v>111.16999999999999</v>
+      </c>
+      <c r="K3">
+        <f>F4</f>
+        <v>111.1</v>
+      </c>
+      <c r="L3" s="13">
+        <f>F22</f>
+        <v>63.23</v>
+      </c>
+      <c r="M3" s="14"/>
+      <c r="O3" s="9">
+        <f>F26</f>
+        <v>47.94</v>
+      </c>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1">
-        <v>222</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F4" s="16">
+        <v>111.1</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="14"/>
+      <c r="K4">
+        <f>F5</f>
+        <v>111.2</v>
+      </c>
+      <c r="L4" s="15">
+        <f>F23</f>
+        <v>47.94</v>
+      </c>
+      <c r="M4" s="14">
+        <v>47.94</v>
+      </c>
+      <c r="O4" s="10">
+        <f>F29</f>
+        <v>43.23</v>
+      </c>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
-        <v>333</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F5" s="16">
+        <v>111.2</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="14">
+        <f>G30</f>
+        <v>43.23</v>
+      </c>
+      <c r="O5" s="10">
+        <v>20</v>
+      </c>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I6" s="15"/>
+      <c r="J6" s="14"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="14">
+        <f>G33</f>
+        <v>20</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="14"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -699,9 +883,14 @@
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="14"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -713,24 +902,39 @@
         <v>111</v>
       </c>
       <c r="D9" s="1">
-        <f>F4</f>
-        <v>222</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <f>F7</f>
+        <v>4</v>
+      </c>
+      <c r="F9" s="18">
+        <v>110102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="14"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>110102.01</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -741,186 +945,208 @@
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="18">
+        <v>110101</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f>A5</f>
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3">
         <v>45139</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="13">
+        <v>20</v>
+      </c>
+      <c r="N13" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f>A2</f>
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3">
         <v>45163</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
         <v>2200025787</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14">
         <v>63.23</v>
       </c>
       <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
         <v>24</v>
       </c>
-      <c r="J14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M14" s="15"/>
+      <c r="N14" s="14"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>45166</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
         <v>172354545</v>
       </c>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H15">
         <v>47.94</v>
       </c>
       <c r="I15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="M15" s="15"/>
+      <c r="N15" s="14"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3">
         <v>45166</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="15"/>
+      <c r="N16" s="14"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C17" s="3">
+        <v>45166</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" s="15"/>
+      <c r="N17" s="14"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <f>F4</f>
-        <v>222</v>
-      </c>
-      <c r="B20" s="1" t="str">
-        <f>G4</f>
-        <v>Propietarios/Arendatarios</v>
-      </c>
-      <c r="C20" s="6" t="str">
+      <c r="G20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="15"/>
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <f>F7</f>
+        <v>4</v>
+      </c>
+      <c r="B21" s="6" t="str">
+        <f>G7</f>
+        <v>Alicuotas</v>
+      </c>
+      <c r="C21" s="6" t="str">
         <f>D13</f>
         <v>Generación de agosto</v>
       </c>
-      <c r="F20" s="1">
-        <f>G21+G22</f>
+      <c r="G21" s="1">
+        <f>F22+F23</f>
         <v>111.16999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <f>F3</f>
-        <v>111</v>
-      </c>
-      <c r="B21" t="str">
-        <f>G3</f>
-        <v>Adeudos Por cobrar</v>
-      </c>
-      <c r="C21" t="str">
-        <f>D13</f>
-        <v>Generación de agosto</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2200025787</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="4">
-        <f>H14</f>
-        <v>63.23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f>F3</f>
         <v>111</v>
@@ -934,70 +1160,72 @@
         <v>Generación de agosto</v>
       </c>
       <c r="D22" s="1">
+        <v>2200025787</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <f>H14</f>
+        <v>63.23</v>
+      </c>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <f>F3</f>
+        <v>111</v>
+      </c>
+      <c r="B23" t="str">
+        <f>G3</f>
+        <v>Adeudos Por cobrar</v>
+      </c>
+      <c r="C23" t="str">
+        <f>D13</f>
+        <v>Generación de agosto</v>
+      </c>
+      <c r="D23" s="1">
         <f>F15</f>
         <v>172354545</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E23" s="1">
         <v>2</v>
       </c>
-      <c r="G22" s="4">
+      <c r="F23" s="4">
         <f>H15</f>
         <v>47.94</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-      <c r="F23">
-        <f>SUM(F20:F22)</f>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+      <c r="F24">
+        <f>SUM(F21:F23)</f>
         <v>111.16999999999999</v>
       </c>
-      <c r="G23">
-        <f>SUM(G20:G22)</f>
+      <c r="G24">
+        <f>SUM(G21:G23)</f>
         <v>111.16999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <f>F5</f>
-        <v>333</v>
-      </c>
-      <c r="B25" s="6" t="str">
-        <f>G5</f>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <f>F10</f>
+        <v>110102.01</v>
+      </c>
+      <c r="B26" s="6" t="str">
+        <f>G10</f>
         <v>Banco Pinchincha</v>
-      </c>
-      <c r="C25" s="1" t="str">
-        <f>D14</f>
-        <v>Pago de Rodrigo Carrión</v>
-      </c>
-      <c r="D25" s="1">
-        <f>F15</f>
-        <v>172354545</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25">
-        <f>H15</f>
-        <v>47.94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <f>F4</f>
-        <v>222</v>
-      </c>
-      <c r="B26" s="6" t="str">
-        <f>$G$4</f>
-        <v>Propietarios/Arendatarios</v>
       </c>
       <c r="C26" s="1" t="str">
         <f>D14</f>
@@ -1007,45 +1235,52 @@
         <f>F15</f>
         <v>172354545</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="G26" s="1">
+      <c r="E26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26">
         <f>H15</f>
         <v>47.94</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <f>$F$5</f>
-        <v>333</v>
-      </c>
-      <c r="B28" t="str">
-        <f>$G$5</f>
+      <c r="H26" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <f>F5</f>
+        <v>111.2</v>
+      </c>
+      <c r="B27" s="6" t="str">
+        <f>G5</f>
+        <v>RODRIGO CARRIÓN</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f>D14</f>
+        <v>Pago de Rodrigo Carrión</v>
+      </c>
+      <c r="D27" s="1">
+        <f>F15</f>
+        <v>172354545</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="G27" s="1">
+        <f>H15</f>
+        <v>47.94</v>
+      </c>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <f>$F$10</f>
+        <v>110102.01</v>
+      </c>
+      <c r="B29" t="str">
+        <f>$G$10</f>
         <v>Banco Pinchincha</v>
-      </c>
-      <c r="C28" t="str">
-        <f>$D$15</f>
-        <v>Pago de Pedro Sandoval</v>
-      </c>
-      <c r="D28" s="1">
-        <f>$F$14</f>
-        <v>2200025787</v>
-      </c>
-      <c r="F28">
-        <f>H14-20</f>
-        <v>43.23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <f>$F$4</f>
-        <v>222</v>
-      </c>
-      <c r="B29" s="6" t="str">
-        <f>$G$4</f>
-        <v>Propietarios/Arendatarios</v>
       </c>
       <c r="C29" t="str">
         <f>$D$15</f>
@@ -1055,45 +1290,49 @@
         <f>$F$14</f>
         <v>2200025787</v>
       </c>
-      <c r="G29">
+      <c r="F29">
+        <f>H14-20</f>
         <v>43.23</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>$F$5</f>
-        <v>333</v>
-      </c>
-      <c r="B31" t="str">
-        <f>$G$5</f>
-        <v>Banco Pinchincha</v>
-      </c>
-      <c r="C31" t="str">
+      <c r="H29" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <f>F4</f>
+        <v>111.1</v>
+      </c>
+      <c r="B30" s="6" t="str">
+        <f>G4</f>
+        <v>PEDRO SANDOVAL</v>
+      </c>
+      <c r="C30" t="str">
         <f>$D$15</f>
         <v>Pago de Pedro Sandoval</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D30" s="1">
         <f>$F$14</f>
         <v>2200025787</v>
       </c>
-      <c r="F31">
-        <f>20</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>43.23</v>
+      </c>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="6"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <f>$F$4</f>
-        <v>222</v>
-      </c>
-      <c r="B32" s="6" t="str">
-        <f>$G$4</f>
-        <v>Propietarios/Arendatarios</v>
+        <f>F12</f>
+        <v>110101</v>
+      </c>
+      <c r="B32" t="str">
+        <f>G12</f>
+        <v>CAJA</v>
       </c>
       <c r="C32" t="str">
         <f>$D$15</f>
@@ -1103,17 +1342,96 @@
         <f>$F$14</f>
         <v>2200025787</v>
       </c>
-      <c r="G32">
+      <c r="F32">
+        <f>20</f>
         <v>20</v>
       </c>
+      <c r="H32" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <f>F4</f>
+        <v>111.1</v>
+      </c>
+      <c r="B33" s="6" t="str">
+        <f>G4</f>
+        <v>PEDRO SANDOVAL</v>
+      </c>
+      <c r="C33" t="str">
+        <f>$D$15</f>
+        <v>Pago de Pedro Sandoval</v>
+      </c>
+      <c r="D33" s="1">
+        <f>$F$14</f>
+        <v>2200025787</v>
+      </c>
+      <c r="G33">
+        <v>20</v>
+      </c>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <f>F10</f>
+        <v>110102.01</v>
+      </c>
+      <c r="B35" t="str">
+        <f>G10</f>
+        <v>Banco Pinchincha</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f>F12</f>
+        <v>110101</v>
+      </c>
+      <c r="B36" t="str">
+        <f>G12</f>
+        <v>CAJA</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36">
+        <v>20</v>
+      </c>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="14">
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
se añade campo para la cuenta contable dentro de departamento
</commit_message>
<xml_diff>
--- a/Prueba Datos Sistema.xlsx
+++ b/Prueba Datos Sistema.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual\Proyecto_Roberto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudio\ProyectoConjuntos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C6A16F-C5EC-4C7E-B1B0-46E2EE33CABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CC95A0-9EFB-4678-9024-9F71C768FB2C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -291,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -328,6 +317,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -350,18 +348,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,10 +363,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,32 +692,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A3F21E-1B0E-4FCA-92AD-C360CB3777B3}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="B1" s="17"/>
+      <c r="F1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -732,21 +730,21 @@
       <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="12" t="str">
+      <c r="I2" s="16" t="str">
         <f>G7</f>
         <v>Alicuotas</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="L2" s="12" t="s">
+      <c r="J2" s="16"/>
+      <c r="L2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="O2" s="12" t="s">
+      <c r="M2" s="16"/>
+      <c r="O2" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="12"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P2" s="16"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -762,8 +760,8 @@
       <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="14">
+      <c r="I3" s="12"/>
+      <c r="J3" s="11">
         <f>F24</f>
         <v>111.16999999999999</v>
       </c>
@@ -771,106 +769,106 @@
         <f>F4</f>
         <v>111.1</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="10">
         <f>F22</f>
         <v>63.23</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="O3" s="9">
+      <c r="M3" s="11"/>
+      <c r="O3" s="7">
         <f>F26</f>
         <v>47.94</v>
       </c>
-      <c r="P3" s="11"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="13">
         <v>111.1</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="14"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="11"/>
       <c r="K4">
         <f>F5</f>
         <v>111.2</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="12">
         <f>F23</f>
         <v>47.94</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="11">
         <v>47.94</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="8">
         <f>F29</f>
         <v>43.23</v>
       </c>
-      <c r="P4" s="11"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <v>111.2</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="14"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="14">
+      <c r="I5" s="12"/>
+      <c r="J5" s="11"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="11">
         <f>G30</f>
         <v>43.23</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="8">
         <v>20</v>
       </c>
-      <c r="P5" s="11"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I6" s="15"/>
-      <c r="J6" s="14"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="14">
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I6" s="12"/>
+      <c r="J6" s="11"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="11">
         <f>G33</f>
         <v>20</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="O6" s="8"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="F7" s="1">
         <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="14"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="14"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I7" s="12"/>
+      <c r="J7" s="11"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="11"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -883,14 +881,14 @@
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="14"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="14"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I8" s="12"/>
+      <c r="J8" s="11"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="11"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -905,20 +903,20 @@
         <f>F7</f>
         <v>4</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="14">
         <v>110102</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="14"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="14"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="11"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I9" s="12"/>
+      <c r="J9" s="11"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="11"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>110102.01</v>
       </c>
@@ -926,15 +924,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -948,18 +946,18 @@
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="18">
+      <c r="F12" s="14">
         <v>110101</v>
       </c>
       <c r="G12" t="s">
         <v>43</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="12"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>A5</f>
         <v>4</v>
@@ -975,14 +973,14 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="M13" s="13">
+      <c r="M13" s="10">
         <v>20</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="11">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>A2</f>
         <v>1</v>
@@ -1015,10 +1013,10 @@
       <c r="K14" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="15"/>
-      <c r="N14" s="14"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M14" s="12"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1044,10 +1042,10 @@
       <c r="I15" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="14"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M15" s="12"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1060,10 +1058,10 @@
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="15"/>
-      <c r="N16" s="14"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M16" s="12"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1076,31 +1074,31 @@
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="14"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M17" s="12"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="14"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="M18" s="12"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="14"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1122,10 +1120,10 @@
       <c r="G20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="15"/>
-      <c r="N20" s="14"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M20" s="12"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>F7</f>
         <v>4</v>
@@ -1142,14 +1140,14 @@
         <f>F22+F23</f>
         <v>111.16999999999999</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f>F3</f>
-        <v>111</v>
+        <f>F4</f>
+        <v>111.1</v>
       </c>
       <c r="B22" t="str">
         <f>G3</f>
@@ -1169,12 +1167,12 @@
         <f>H14</f>
         <v>63.23</v>
       </c>
-      <c r="H22" s="17"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f>F3</f>
-        <v>111</v>
+        <f>F5</f>
+        <v>111.2</v>
       </c>
       <c r="B23" t="str">
         <f>G3</f>
@@ -1195,9 +1193,9 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="F24">
         <f>SUM(F21:F23)</f>
@@ -1207,18 +1205,21 @@
         <f>SUM(G21:G23)</f>
         <v>111.16999999999999</v>
       </c>
-      <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="7" t="s">
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f>F10</f>
         <v>110102.01</v>
@@ -1242,11 +1243,11 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>F5</f>
         <v>111.2</v>
@@ -1268,12 +1269,12 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f>$F$10</f>
         <v>110102.01</v>
@@ -1294,11 +1295,11 @@
         <f>H14-20</f>
         <v>43.23</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f>F4</f>
         <v>111.1</v>
@@ -1318,14 +1319,14 @@
       <c r="G30">
         <v>43.23</v>
       </c>
-      <c r="H30" s="17"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="6"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>F12</f>
         <v>110101</v>
@@ -1346,11 +1347,11 @@
         <f>20</f>
         <v>20</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f>F4</f>
         <v>111.1</v>
@@ -1370,9 +1371,9 @@
       <c r="G33">
         <v>20</v>
       </c>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="15"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f>F10</f>
         <v>110102.01</v>
@@ -1387,11 +1388,11 @@
       <c r="F35">
         <v>20</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H35" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>F12</f>
         <v>110101</v>
@@ -1406,9 +1407,9 @@
       <c r="G36">
         <v>20</v>
       </c>
-      <c r="H36" s="17"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="15"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>49</v>
       </c>
@@ -1417,7 +1418,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="M12:N12"/>
@@ -1426,12 +1434,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="H21:H24"/>
     <mergeCell ref="H26:H27"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Inicio de guardar cabecera cuando se crea el adeudo
</commit_message>
<xml_diff>
--- a/Prueba Datos Sistema.xlsx
+++ b/Prueba Datos Sistema.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudio\ProyectoConjuntos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VisualStudio\Personal\Roberto-Conjuntos\ProyectoConjuntos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A88D8F-5D82-45AD-8E40-DCE250651DC7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8512B017-9979-49C5-A89E-8372BB0A942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
+    <workbookView xWindow="3945" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>Ingreso</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Ctas.por Cobrar Clientes</t>
+  </si>
+  <si>
+    <t>GeneraciónAdeudo</t>
   </si>
 </sst>
 </file>
@@ -321,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,11 +347,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -357,15 +356,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,7 +682,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,14 +697,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="F1" s="18" t="s">
+      <c r="B1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="18"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -721,19 +719,19 @@
       <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="17" t="str">
+      <c r="I2" s="14" t="str">
         <f>G7</f>
         <v>Alicuotas</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="L2" s="17" t="s">
+      <c r="J2" s="14"/>
+      <c r="L2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="O2" s="17" t="s">
+      <c r="M2" s="14"/>
+      <c r="O2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="17"/>
+      <c r="P2" s="14"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -751,8 +749,8 @@
       <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="12">
+      <c r="I3" s="11"/>
+      <c r="J3" s="1">
         <f>F24</f>
         <v>111.16999999999999</v>
       </c>
@@ -760,16 +758,15 @@
         <f>F4</f>
         <v>113.1</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <f>F22</f>
         <v>63.23</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="1"/>
       <c r="O3" s="8">
         <f>F26</f>
         <v>47.94</v>
       </c>
-      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -778,86 +775,82 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <v>113.1</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="12"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="1"/>
       <c r="K4">
         <f>F5</f>
         <v>113.2</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="11">
         <f>F23</f>
         <v>47.94</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="1">
         <v>47.94</v>
       </c>
       <c r="O4" s="9">
         <f>F29</f>
         <v>43.23</v>
       </c>
-      <c r="P4" s="10"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="14">
+        <v>51</v>
+      </c>
+      <c r="F5" s="12">
         <v>113.2</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="12"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="12">
+      <c r="I5" s="11"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="1">
         <f>G30</f>
         <v>43.23</v>
       </c>
       <c r="O5" s="9">
         <v>20</v>
       </c>
-      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I6" s="13"/>
-      <c r="J6" s="12"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="12">
+      <c r="I6" s="11"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="1">
         <f>G33</f>
         <v>20</v>
       </c>
       <c r="O6" s="9"/>
-      <c r="P6" s="10"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="F7" s="1">
         <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="12"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="1"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -872,12 +865,11 @@
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="12"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="1"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="1"/>
       <c r="O8" s="9"/>
-      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -894,18 +886,17 @@
         <f>F7</f>
         <v>4</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9">
         <v>110102</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="12"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="12"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="1"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="1"/>
       <c r="O9" s="9"/>
-      <c r="P9" s="10"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F10">
@@ -916,12 +907,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -937,16 +928,16 @@
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="15">
+      <c r="F12">
         <v>110101</v>
       </c>
       <c r="G12" t="s">
         <v>43</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="17"/>
+      <c r="N12" s="14"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -964,10 +955,10 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="M13" s="11">
+      <c r="M13" s="10">
         <v>20</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="1">
         <v>20</v>
       </c>
     </row>
@@ -1004,8 +995,8 @@
       <c r="K14" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="13"/>
-      <c r="N14" s="12"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1033,8 +1024,8 @@
       <c r="I15" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="12"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1049,8 +1040,8 @@
       <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="13"/>
-      <c r="N16" s="12"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1065,29 +1056,29 @@
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="13"/>
-      <c r="N17" s="12"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="12"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1111,8 +1102,8 @@
       <c r="G20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="13"/>
-      <c r="N20" s="12"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="1"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1131,7 +1122,7 @@
         <f>F22+F23</f>
         <v>111.16999999999999</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1158,7 +1149,7 @@
         <f>H14</f>
         <v>63.23</v>
       </c>
-      <c r="H22" s="16"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1184,7 +1175,7 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H23" s="16"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
@@ -1196,7 +1187,7 @@
         <f>SUM(G21:G23)</f>
         <v>111.16999999999999</v>
       </c>
-      <c r="H24" s="16"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1231,7 +1222,7 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1257,7 +1248,7 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H27" s="16"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
@@ -1283,7 +1274,7 @@
         <f>H14-20</f>
         <v>43.23</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1307,7 +1298,7 @@
       <c r="G30">
         <v>43.23</v>
       </c>
-      <c r="H30" s="16"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -1335,7 +1326,7 @@
         <f>20</f>
         <v>20</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H32" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1359,7 +1350,7 @@
       <c r="G33">
         <v>20</v>
       </c>
-      <c r="H33" s="16"/>
+      <c r="H33" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -1376,7 +1367,7 @@
       <c r="F35">
         <v>20</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H35" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1395,7 +1386,7 @@
       <c r="G36">
         <v>20</v>
       </c>
-      <c r="H36" s="16"/>
+      <c r="H36" s="15"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
@@ -1407,12 +1398,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="M12:N12"/>
@@ -1421,6 +1406,12 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="H21:H24"/>
     <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Guardar registro cabecera contablr
</commit_message>
<xml_diff>
--- a/Prueba Datos Sistema.xlsx
+++ b/Prueba Datos Sistema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VisualStudio\Personal\Roberto-Conjuntos\ProyectoConjuntos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8512B017-9979-49C5-A89E-8372BB0A942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E696D8C-011D-4F8C-9519-3CC65496CDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
+    <workbookView xWindow="-10425" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{3156AAED-AD50-4D70-98B1-0E489F982C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -356,14 +356,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,7 +682,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A13" sqref="A13:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,14 +697,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -834,12 +834,12 @@
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
       <c r="F7" s="1">
         <v>4</v>
       </c>
@@ -907,12 +907,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1068,15 +1068,15 @@
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
       <c r="M19" s="11"/>
       <c r="N19" s="1"/>
     </row>
@@ -1122,7 +1122,7 @@
         <f>F22+F23</f>
         <v>111.16999999999999</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
         <f>H14</f>
         <v>63.23</v>
       </c>
-      <c r="H22" s="15"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1175,7 +1175,7 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H23" s="15"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
@@ -1187,7 +1187,7 @@
         <f>SUM(G21:G23)</f>
         <v>111.16999999999999</v>
       </c>
-      <c r="H24" s="15"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1222,7 +1222,7 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1248,7 +1248,7 @@
         <f>H15</f>
         <v>47.94</v>
       </c>
-      <c r="H27" s="15"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
@@ -1274,7 +1274,7 @@
         <f>H14-20</f>
         <v>43.23</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1298,7 +1298,7 @@
       <c r="G30">
         <v>43.23</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -1326,7 +1326,7 @@
         <f>20</f>
         <v>20</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1350,7 +1350,7 @@
       <c r="G33">
         <v>20</v>
       </c>
-      <c r="H33" s="15"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -1367,7 +1367,7 @@
       <c r="F35">
         <v>20</v>
       </c>
-      <c r="H35" s="15" t="s">
+      <c r="H35" s="13" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       <c r="G36">
         <v>20</v>
       </c>
-      <c r="H36" s="15"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
@@ -1398,6 +1398,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="H29:H30"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="M12:N12"/>
@@ -1406,12 +1412,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="H21:H24"/>
     <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>